<commit_message>
Updated Lab inventory and added list of electronic componets to buy
</commit_message>
<xml_diff>
--- a/to_buy/Lab_Inventory.xlsx
+++ b/to_buy/Lab_Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>Part</t>
   </si>
@@ -478,6 +478,15 @@
   </si>
   <si>
     <t>Want at least 1 for each group in a lab section. I think the link is to the same brand of speakers</t>
+  </si>
+  <si>
+    <t>Table Clamp</t>
+  </si>
+  <si>
+    <t>IR Sensor cables</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/117</t>
   </si>
 </sst>
 </file>
@@ -804,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1413,42 +1422,36 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>153</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56">
-        <v>10</v>
-      </c>
-      <c r="C56">
-        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57" t="s">
-        <v>96</v>
-      </c>
-      <c r="E57" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1457,138 +1460,141 @@
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="E58" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="B59">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
-        <v>98</v>
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B61">
-        <v>8</v>
-      </c>
-      <c r="C61">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="E62" t="s">
-        <v>99</v>
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B63">
-        <v>4</v>
-      </c>
-      <c r="C63">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>70</v>
       </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68">
-        <v>2</v>
-      </c>
-      <c r="E68" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71">
-        <v>3</v>
-      </c>
-      <c r="E71" t="s">
-        <v>118</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -1596,50 +1602,56 @@
       <c r="C72">
         <v>3</v>
       </c>
+      <c r="E72" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>41</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>42</v>
       </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>50</v>
-      </c>
-      <c r="B76">
-        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B77">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -1647,40 +1659,37 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B80">
-        <v>1</v>
-      </c>
-      <c r="C80">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B81">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C81">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B82">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B83">
         <v>2</v>
@@ -1691,296 +1700,324 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B84">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C84">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>68</v>
+      </c>
+      <c r="B85">
+        <v>14</v>
+      </c>
+      <c r="C85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>69</v>
       </c>
-      <c r="B85">
-        <v>1</v>
-      </c>
-      <c r="C85">
-        <v>2</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>73</v>
-      </c>
-      <c r="B88">
-        <v>2</v>
-      </c>
-      <c r="C88">
-        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C89">
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B90">
-        <v>4</v>
-      </c>
-      <c r="C90">
-        <v>5</v>
-      </c>
-      <c r="D90" t="s">
-        <v>86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B91">
+        <v>4</v>
+      </c>
+      <c r="C91">
         <v>5</v>
+      </c>
+      <c r="D91" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B92">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>77</v>
+      </c>
+      <c r="B93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>83</v>
       </c>
-      <c r="B93">
+      <c r="B94">
         <v>0</v>
       </c>
-      <c r="C93">
+      <c r="C94">
         <v>5</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>85</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E94" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>121</v>
-      </c>
-      <c r="B96">
-        <v>8</v>
-      </c>
-      <c r="C96">
-        <v>15</v>
-      </c>
-      <c r="E96" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B97">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C97">
-        <v>36</v>
-      </c>
-      <c r="D97" t="s">
-        <v>135</v>
+        <v>15</v>
+      </c>
+      <c r="E97" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B98">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C98">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B99">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C99">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="D99" t="s">
-        <v>137</v>
-      </c>
-      <c r="E99" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B100">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C100">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="D100" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="E100" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B101">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C101">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D101" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="B102">
+        <v>33</v>
       </c>
       <c r="C102">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D102" t="s">
-        <v>140</v>
-      </c>
-      <c r="E102" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>128</v>
-      </c>
-      <c r="B103">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="C103">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D103" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="E103" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="B104">
+        <v>37</v>
       </c>
       <c r="C104">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D104" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B105">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C105">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B106">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="C106">
+        <v>24</v>
       </c>
       <c r="D106" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B107">
-        <v>32</v>
-      </c>
-      <c r="C107">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B108">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C108">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D108" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C109">
         <v>24</v>
       </c>
       <c r="D109" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>145</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>24</v>
+      </c>
+      <c r="D110" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>154</v>
+      </c>
+      <c r="B111">
+        <v>12</v>
+      </c>
+      <c r="C111">
+        <v>100</v>
+      </c>
+      <c r="D111" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>